<commit_message>
Excel data for login
</commit_message>
<xml_diff>
--- a/Excel/LoginInfo.xlsx
+++ b/Excel/LoginInfo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/65b3116eb161f8cf/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/65b3116eb161f8cf/מסמכים/GitHub/QA-project/QA-project/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_F25DC773A252ABDACC1048EBA11F51C65BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21235362-FA5A-4540-B342-9279216553F5}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="11_F25DC773A252ABDACC1048EBA11F51C65BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AA14A40-3358-488F-BAC0-E99BF8FE178D}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26475" yWindow="0" windowWidth="25125" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -49,6 +49,15 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>Yam</t>
+  </si>
+  <si>
+    <t>afasfasf</t>
+  </si>
+  <si>
+    <t>Yam biton</t>
   </si>
 </sst>
 </file>
@@ -59,7 +68,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -105,7 +114,7 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{9F29198A-9CCC-47A7-94C5-0911BFD1042C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="5">
+  <queryTableRefresh nextId="7">
     <queryTableFields count="4">
       <queryTableField id="1" name="Name" tableColumnId="1"/>
       <queryTableField id="2" name="Username" tableColumnId="2"/>
@@ -405,21 +414,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{901EC5C4-B4DE-469B-A068-8E5576BCED1C}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.921875" customWidth="1"/>
-    <col min="2" max="2" width="22.921875" customWidth="1"/>
-    <col min="3" max="3" width="19.4609375" customWidth="1"/>
-    <col min="4" max="4" width="35.921875" customWidth="1"/>
+    <col min="1" max="1" width="17.875" customWidth="1"/>
+    <col min="2" max="2" width="22.875" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="35.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,6 +440,20 @@
       </c>
       <c r="D1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>123456789</v>
       </c>
     </row>
   </sheetData>
@@ -449,13 +472,13 @@
       <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.15234375" customWidth="1"/>
-    <col min="4" max="4" width="10.61328125" customWidth="1"/>
+    <col min="2" max="2" width="11.125" customWidth="1"/>
+    <col min="4" max="4" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>

</xml_diff>